<commit_message>
Fix wrong text alignment in cells
</commit_message>
<xml_diff>
--- a/template_outside.xlsx
+++ b/template_outside.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\magneto\home\Dokumente\_Sonstiges\Ordnung\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\magneto\home\Dokumente\_Sonstiges\Ordnung\assortment-box-lables\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,10 +21,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -182,56 +178,47 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -524,382 +511,382 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="15"/>
+      <c r="A1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="16"/>
+      <c r="A2" s="1"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="12"/>
+      <c r="A3" s="1"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="12"/>
+      <c r="A4" s="1"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="13"/>
+      <c r="A5" s="1"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="2"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="10"/>
     </row>
     <row r="7" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="15"/>
+      <c r="A7" s="5"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="16"/>
+      <c r="A8" s="1"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="12"/>
+      <c r="A9" s="1"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="12"/>
+      <c r="A10" s="1"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="13"/>
+      <c r="A11" s="1"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="2"/>
+      <c r="A12" s="10"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="10"/>
     </row>
     <row r="13" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="15"/>
+      <c r="A13" s="5"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="16"/>
-    </row>
-    <row r="15" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A15" s="20"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="20"/>
-    </row>
-    <row r="16" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A16" s="20"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="20"/>
-    </row>
-    <row r="17" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A17" s="20"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="20"/>
+      <c r="A14" s="1"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="13"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="13"/>
+    </row>
+    <row r="16" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="13"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="13"/>
+    </row>
+    <row r="17" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="13"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="13"/>
     </row>
     <row r="18" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="2"/>
+      <c r="A18" s="10"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="10"/>
     </row>
     <row r="19" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="15"/>
+      <c r="A19" s="5"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="5"/>
     </row>
     <row r="20" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="16"/>
+      <c r="A20" s="1"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="1"/>
     </row>
     <row r="21" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="12"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="12"/>
+      <c r="A21" s="1"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="12"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="12"/>
+      <c r="A22" s="1"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="1"/>
     </row>
     <row r="23" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="16"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="13"/>
+      <c r="A23" s="1"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="1"/>
     </row>
     <row r="24" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="14"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="2"/>
+      <c r="A24" s="10"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="10"/>
     </row>
     <row r="25" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="15"/>
+      <c r="A25" s="5"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="5"/>
     </row>
     <row r="26" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="13"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="16"/>
+      <c r="A26" s="1"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="1"/>
     </row>
     <row r="27" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="12"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="12"/>
+      <c r="A27" s="1"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="1"/>
     </row>
     <row r="28" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="12"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="12"/>
+      <c r="A28" s="1"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="1"/>
     </row>
     <row r="29" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="16"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="13"/>
+      <c r="A29" s="1"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="1"/>
     </row>
     <row r="30" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="14"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="2"/>
+      <c r="A30" s="10"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="10"/>
     </row>
     <row r="31" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="15"/>
+      <c r="A31" s="5"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="5"/>
     </row>
     <row r="32" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="13"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="16"/>
+      <c r="A32" s="1"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="1"/>
     </row>
     <row r="33" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="12"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="12"/>
+      <c r="A33" s="1"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="1"/>
     </row>
     <row r="34" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="12"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="12"/>
+      <c r="A34" s="1"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="1"/>
     </row>
     <row r="35" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="16"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="13"/>
+      <c r="A35" s="1"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="1"/>
     </row>
     <row r="36" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="14"/>
-      <c r="B36" s="5"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="2"/>
+      <c r="A36" s="10"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="10"/>
     </row>
     <row r="37" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="17"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="15"/>
+      <c r="A37" s="5"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="5"/>
     </row>
     <row r="38" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="13"/>
-      <c r="B38" s="4"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="10"/>
-      <c r="E38" s="16"/>
-    </row>
-    <row r="39" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A39" s="20"/>
-      <c r="B39" s="4"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="20"/>
-    </row>
-    <row r="40" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A40" s="20"/>
-      <c r="B40" s="4"/>
-      <c r="C40" s="18"/>
-      <c r="D40" s="10"/>
-      <c r="E40" s="20"/>
-    </row>
-    <row r="41" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A41" s="20"/>
-      <c r="B41" s="4"/>
-      <c r="C41" s="18"/>
-      <c r="D41" s="10"/>
-      <c r="E41" s="20"/>
+      <c r="A38" s="1"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="1"/>
+    </row>
+    <row r="39" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="13"/>
+      <c r="B39" s="8"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="13"/>
+    </row>
+    <row r="40" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="13"/>
+      <c r="B40" s="8"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="13"/>
+    </row>
+    <row r="41" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="13"/>
+      <c r="B41" s="8"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="13"/>
     </row>
     <row r="42" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="14"/>
-      <c r="B42" s="5"/>
-      <c r="C42" s="19"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="2"/>
+      <c r="A42" s="10"/>
+      <c r="B42" s="11"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="10"/>
     </row>
     <row r="43" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="1"/>
-      <c r="B43" s="3"/>
-      <c r="C43" s="6"/>
-      <c r="D43" s="9"/>
-      <c r="E43" s="15"/>
+      <c r="A43" s="5"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="5"/>
     </row>
     <row r="44" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="13"/>
-      <c r="B44" s="4"/>
-      <c r="C44" s="7"/>
-      <c r="D44" s="10"/>
-      <c r="E44" s="16"/>
+      <c r="A44" s="1"/>
+      <c r="B44" s="8"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="1"/>
     </row>
     <row r="45" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="12"/>
-      <c r="B45" s="4"/>
-      <c r="C45" s="7"/>
-      <c r="D45" s="10"/>
-      <c r="E45" s="12"/>
+      <c r="A45" s="1"/>
+      <c r="B45" s="8"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="1"/>
     </row>
     <row r="46" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="12"/>
-      <c r="B46" s="4"/>
-      <c r="C46" s="7"/>
-      <c r="D46" s="10"/>
-      <c r="E46" s="12"/>
+      <c r="A46" s="1"/>
+      <c r="B46" s="8"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="1"/>
     </row>
     <row r="47" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="16"/>
-      <c r="B47" s="4"/>
-      <c r="C47" s="7"/>
-      <c r="D47" s="10"/>
-      <c r="E47" s="13"/>
+      <c r="A47" s="1"/>
+      <c r="B47" s="8"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="1"/>
     </row>
     <row r="48" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="14"/>
-      <c r="B48" s="5"/>
-      <c r="C48" s="8"/>
-      <c r="D48" s="11"/>
-      <c r="E48" s="2"/>
+      <c r="A48" s="10"/>
+      <c r="B48" s="11"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="12"/>
+      <c r="E48" s="10"/>
     </row>
     <row r="49" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="1"/>
-      <c r="B49" s="3"/>
-      <c r="C49" s="6"/>
-      <c r="D49" s="9"/>
-      <c r="E49" s="15"/>
+      <c r="A49" s="5"/>
+      <c r="B49" s="6"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="5"/>
     </row>
     <row r="50" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="13"/>
-      <c r="B50" s="4"/>
-      <c r="C50" s="7"/>
-      <c r="D50" s="10"/>
-      <c r="E50" s="16"/>
+      <c r="A50" s="1"/>
+      <c r="B50" s="8"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="1"/>
     </row>
     <row r="51" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="12"/>
-      <c r="B51" s="4"/>
-      <c r="C51" s="7"/>
-      <c r="D51" s="10"/>
-      <c r="E51" s="12"/>
+      <c r="A51" s="1"/>
+      <c r="B51" s="8"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="1"/>
     </row>
     <row r="52" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="12"/>
-      <c r="B52" s="4"/>
-      <c r="C52" s="7"/>
-      <c r="D52" s="10"/>
-      <c r="E52" s="12"/>
+      <c r="A52" s="1"/>
+      <c r="B52" s="8"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="1"/>
     </row>
     <row r="53" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="16"/>
-      <c r="B53" s="4"/>
-      <c r="C53" s="7"/>
-      <c r="D53" s="10"/>
-      <c r="E53" s="13"/>
+      <c r="A53" s="1"/>
+      <c r="B53" s="8"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="1"/>
     </row>
     <row r="54" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="14"/>
-      <c r="B54" s="5"/>
-      <c r="C54" s="8"/>
-      <c r="D54" s="11"/>
-      <c r="E54" s="2"/>
+      <c r="A54" s="10"/>
+      <c r="B54" s="11"/>
+      <c r="C54" s="4"/>
+      <c r="D54" s="12"/>
+      <c r="E54" s="10"/>
     </row>
     <row r="55" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="56" spans="1:5" ht="14.1" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>